<commit_message>
Fixed failures in Selendroid
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/Webview_Ruby.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/Webview_Ruby.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="85">
   <si>
     <t>Testcase ID</t>
   </si>
@@ -429,14 +429,603 @@
 ClickRunTest(runtest_top_xpath);
 validate3;
 ClickRunTest(runtest_bottom_xpath);
+wait(2);
+SwitchApp(NATIVE_APP);
+wait(2);
+ClickNativeIcon(VT200_0976_tab1_xpath);
+wait(2);
+ClickNativeIcon(VT200_0976_tab0_xpath);
+wait(2);
+SwitchApp(WEBVIEW);
+wait(2);
+SelectTestToRun(VT200_0985_string);
+ClickRunTest(runtest_top_xpath);
+validate4;
+ClickRunTest(runtest_bottom_xpath);
 wait(3);
 SwitchApp(NATIVE_APP);
 wait(2);
 ClickNativeIcon(VT200_0976_tab1_xpath);
-wait(2);
+wait(5);
+CheckUITextContains(Google);
 ClickNativeIcon(VT200_0976_tab0_xpath);
 wait(2);
 SwitchApp(WEBVIEW);
+wait(2);
+ScrollUp_Page(body_xpath);
+SelectTestToRun(VT200_0986_string);
+ClickRunTest(runtest_top_xpath);
+validate6;
+ClickRunTest(runtest_bottom_xpath);
+wait(3);
+SwitchApp(NATIVE_APP);
+wait(2);
+ClickNativeIcon(VT200_0976_tab1_xpath);
+wait(4);
+CheckUITextContains(Page1);</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(webview_test_link);
+validate2;
+SelectTestToRun(VT200_0976_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+SwitchApp(NATIVE_APP);
+wait(2);
+ClickNativeIcon(VT200_0976_tab1_xpath);
+wait(10);
+TakeScreenshot(VT200_0987_before);
+validate5;
+ClickNativeIcon(VT200_0976_tab0_xpath);
+wait(2);
+SwitchApp(WEBVIEW);
+wait(2);
+SelectTestToRun(VT200_0987_string);
+ClickRunTest(runtest_top_xpath);
+validate6;
+ClickRunTest(runtest_bottom_xpath);
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(VT200_0976_tab1_xpath);
+TakeScreenshot(VT200_0987_after);
+validate7;</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(webview_test_link);
+validate2;
+SelectTestToRun(VT200_0995_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(2);
+validate4;
+TakeScreenshot(VT200_0995);
+wait(2);
+validate5;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Manual Compliance Ruby Specs
+};
+validate2
+{
+validate_PageTitle=Webview Ruby Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0993
+};
+validate4
+{
+validate_Result=true
+};
+validate5
+{
+validate_Screenshot=VT200_0993_before
+};
+validate6
+{
+validate_Screenshot=VT200_0993_after
+};</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate1
+{
+validate_PageTitle=Manual Compliance Ruby Specs
+};
+validate2
+{
+validate_PageTitle=Webview Ruby Test
+};
+validate3
+{
+validate_Text_Exists=VT200-1002
+};
+validate4
+{
+validate_Result=1. enable_screen_zoom set value is 0
+validate_Result=2. WebView enableZoom value is true
+};
+</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Manual Compliance Ruby Specs
+};
+validate2
+{
+validate_PageTitle=Webview Ruby Test
+};
+validate3
+{
+validate_Text_Exists=VT200-1002
+};
+validate4
+{
+validate_Result=1. enable_screen_zoom set value is 0
+validate_Result=2. WebView enableZoom value is false
+};
+validate5
+{
+validate_Screenshot=VT200_1002_before
+validate_Screenshot=VT200-1002
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Manual Compliance Ruby Specs
+};
+validate2
+{
+validate_PageTitle=Webview Ruby Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0976
+};
+validate5
+{
+validate_Screenshot=VT200_0987_before
+};
+validate6
+{
+validate_Text_Exists=VT200-0987
+};
+validate7
+{
+validate_Screenshot=VT200_0987_after
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Manual Compliance Ruby Specs
+};
+validate2
+{
+validate_PageTitle=Webview Ruby Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0994
+};
+validate4
+{
+validate_Result=false
+};
+validate5
+{
+validate_Screenshot=VT200_0994
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Manual Compliance Ruby Specs
+};
+validate2
+{
+validate_PageTitle=Webview Ruby Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0995
+};
+validate4
+{
+validate_Result=true
+};
+validate5
+{
+validate_Screenshot=VT200_0995
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Manual Compliance Ruby Specs
+};
+validate2
+{
+validate_PageTitle=Webview Ruby Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0999
+};
+validate4
+{
+validate_Result=true
+};
+validate5
+{
+validate_Screenshot=VT200_0999
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Manual Compliance Ruby Specs
+};
+validate2
+{
+validate_PageTitle=Webview Ruby Test
+};
+validate3
+{
+validate_Text_Exists=VT200-1000
+};
+validate4
+{
+validate_Result=true
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Manual Compliance Ruby Specs
+};
+validate2
+{
+validate_PageTitle=Webview Ruby Test
+};
+validate3
+{
+validate_Text_Exists=VT200-1000
+};
+validate4
+{
+validate_Result=false
+};
+validate5
+{
+validate_Screenshot=VT200_1000
+};</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate1
+{
+validate_PageTitle=Manual Compliance Ruby Specs
+};
+validate2
+{
+validate_PageTitle=Webview Ruby Test
+};
+validate3
+{
+validate_Text_Exists=VT200-1003
+};
+validate4
+{
+validate_Result=true
+};
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate1
+{
+validate_PageTitle=Manual Compliance Ruby Specs
+};
+validate2
+{
+validate_PageTitle=Webview Ruby Test
+};
+validate3
+{
+validate_Text_Exists=VT200-1004
+};
+validate4
+{
+validate_Result=1. enable_web_plugins set value is 0
+validate_Result=2. WebView enableWebPlugins value is true
+};
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate1
+{
+validate_PageTitle=Manual Compliance Ruby Specs
+};
+validate2
+{
+validate_PageTitle=Webview Ruby Test
+};
+validate3
+{
+validate_Text_Exists=VT200-1004
+};
+validate4
+{
+validate_Result=1. enable_web_plugins set value is 0
+validate_Result=2. WebView enableWebPlugins value is false
+};
+</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Manual Compliance Ruby Specs
+};
+validate2
+{
+validate_PageTitle=Webview Ruby Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0976
+};
+validate5
+{
+validate_Text_Exists=VT200-0978
+};
+validate6
+{
+validate_Result=http://127.0.0.1
+validate_Result=app/WebviewNew/Page4.html
+};</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate1
+{
+validate_PageTitle=Manual Compliance Ruby Specs
+};
+validate2
+{
+validate_PageTitle=Webview Ruby Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0980
+};
+validate5
+{
+validate_Alert=Hello
+};
+</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Manual Compliance Ruby Specs
+};
+validate2
+{
+validate_PageTitle=Webview Ruby Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0976
+};
+validate4
+{
+validate_Text_Exists=VT200-0981
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Manual Compliance Ruby Specs
+};
+validate2
+{
+validate_PageTitle=Webview Ruby Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0976
+};
+validate4
+{
+validate_Text_Exists=VT200-0985
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Manual Compliance Ruby Specs
+};
+validate2
+{
+validate_PageTitle=Webview Ruby Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0976
+};
+validate4
+{
+validate_Text_Exists=VT200-0985
+};
+validate6
+{
+validate_Text_Exists=VT200-0986
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Manual Compliance Ruby Specs
+};
+validate2
+{
+validate_PageTitle=Webview Ruby Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0976
+};
+validate4
+{
+validate_Text_Exists=VT200-0983
+};
+validate5
+{
+validate_Result=true
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Manual Compliance Ruby Specs
+};
+validate2
+{
+validate_PageTitle=Webview Ruby Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0991
+};
+validate4
+{
+validate_SystemProperties=webviewFramework
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Manual Compliance Ruby Specs
+};
+validate2
+{
+validate_PageTitle=Webview Ruby Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0988
+};
+validate4
+{
+validate_Result=true
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Manual Compliance Ruby Specs
+};
+validate2
+{
+validate_PageTitle=Webview Ruby Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0989
+};
+validate4
+{
+validate_Result=true
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Manual Compliance Ruby Specs
+};
+validate2
+{
+validate_PageTitle=Webview Ruby Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0990
+};
+validate4
+{
+validate_Result=true
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Manual Compliance Ruby Specs
+};
+validate2
+{
+validate_PageTitle=Webview Ruby Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0990
+};
+validate4
+{
+validate_Result=false
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Manual Compliance Ruby Specs
+};
+validate2
+{
+validate_PageTitle=Webview Ruby Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0976
+};
+validate4
+{
+validate_Text_Exists=VT200-0979
+};
+validate5
+{
+validate_Result=http://127.0.0.1:
+validate_Result=app/Webview/Page1.html
+};</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(webview_test_link);
+validate2;
+SelectTestToRun(VT200_0976_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(3);
+SwitchApp(NATIVE_APP);
+wait(2);
+ClickNativeIcon(VT200_0976_tab1_xpath);
+wait(2);
+ClickNativeIcon(VT200_0976_tab0_xpath);
+wait(2);
+SwitchApp(WEBVIEW);
+wait(2);
+SelectTestToRun(VT200_0983_string);
+ClickRunTest(runtest_top_xpath);
+wait(3);
+validate4;
+ClickRunTest(runtest_bottom_xpath);
 wait(2);
 SelectTestToRun(VT200_0983_string);
 ClickRunTest(runtest_top_xpath);
@@ -469,97 +1058,10 @@
 validate4;
 ClickRunTest(runtest_bottom_xpath);
 wait(5);
-validate5;
+CheckUITextContains(Active_Tab_is:_1);
 </t>
   </si>
   <si>
-    <t>wait(3);
-validate1;
-link_Click(webview_test_link);
-validate2;
-SelectTestToRun(VT200_0976_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-wait(2);
-SwitchApp(NATIVE_APP);
-wait(2);
-ClickNativeIcon(VT200_0976_tab1_xpath);
-wait(2);
-ClickNativeIcon(VT200_0976_tab0_xpath);
-wait(2);
-SwitchApp(WEBVIEW);
-wait(2);
-SelectTestToRun(VT200_0985_string);
-ClickRunTest(runtest_top_xpath);
-validate4;
-ClickRunTest(runtest_bottom_xpath);
-wait(3);
-SwitchApp(NATIVE_APP);
-wait(2);
-ClickNativeIcon(VT200_0976_tab1_xpath);
-wait(5);
-CheckUITextContains(Google);
-ClickNativeIcon(VT200_0976_tab0_xpath);
-wait(2);
-SwitchApp(WEBVIEW);
-wait(2);
-ScrollUp_Page(body_xpath);
-SelectTestToRun(VT200_0986_string);
-ClickRunTest(runtest_top_xpath);
-validate6;
-ClickRunTest(runtest_bottom_xpath);
-wait(3);
-SwitchApp(NATIVE_APP);
-wait(2);
-ClickNativeIcon(VT200_0976_tab1_xpath);
-wait(4);
-CheckUITextContains(Page1);</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-link_Click(webview_test_link);
-validate2;
-SelectTestToRun(VT200_0976_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-SwitchApp(NATIVE_APP);
-wait(2);
-ClickNativeIcon(VT200_0976_tab1_xpath);
-wait(10);
-TakeScreenshot(VT200_0987_before);
-validate5;
-ClickNativeIcon(VT200_0976_tab0_xpath);
-wait(2);
-SwitchApp(WEBVIEW);
-wait(2);
-SelectTestToRun(VT200_0987_string);
-ClickRunTest(runtest_top_xpath);
-validate6;
-ClickRunTest(runtest_bottom_xpath);
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(VT200_0976_tab1_xpath);
-TakeScreenshot(VT200_0987_after);
-validate7;</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-link_Click(webview_test_link);
-validate2;
-SelectTestToRun(VT200_0995_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-wait(2);
-validate4;
-TakeScreenshot(VT200_0995);
-wait(2);
-validate5;</t>
-  </si>
-  <si>
     <t>validate1
 {
 validate_PageTitle=Manual Compliance Ruby Specs
@@ -570,525 +1072,18 @@
 };
 validate3
 {
-validate_Text_Exists=VT200-0993
+validate_Text_Exists=VT200-0976
 };
 validate4
 {
-validate_Result=true
-};
-validate5
-{
-validate_Screenshot=VT200_0993_before
-};
-validate6
-{
-validate_Screenshot=VT200_0993_after
+validate_Text_Exists=VT200-0977
 };</t>
-  </si>
-  <si>
-    <t xml:space="preserve">validate1
-{
-validate_PageTitle=Manual Compliance Ruby Specs
-};
-validate2
-{
-validate_PageTitle=Webview Ruby Test
-};
-validate3
-{
-validate_Text_Exists=VT200-1002
-};
-validate4
-{
-validate_Result=1. enable_screen_zoom set value is 0
-validate_Result=2. WebView enableZoom value is true
-};
-</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Manual Compliance Ruby Specs
-};
-validate2
-{
-validate_PageTitle=Webview Ruby Test
-};
-validate3
-{
-validate_Text_Exists=VT200-1002
-};
-validate4
-{
-validate_Result=1. enable_screen_zoom set value is 0
-validate_Result=2. WebView enableZoom value is false
-};
-validate5
-{
-validate_Screenshot=VT200_1002_before
-validate_Screenshot=VT200-1002
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Manual Compliance Ruby Specs
-};
-validate2
-{
-validate_PageTitle=Webview Ruby Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0976
-};
-validate5
-{
-validate_Screenshot=VT200_0987_before
-};
-validate6
-{
-validate_Text_Exists=VT200-0987
-};
-validate7
-{
-validate_Screenshot=VT200_0987_after
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Manual Compliance Ruby Specs
-};
-validate2
-{
-validate_PageTitle=Webview Ruby Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0994
-};
-validate4
-{
-validate_Result=false
-};
-validate5
-{
-validate_Screenshot=VT200_0994
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Manual Compliance Ruby Specs
-};
-validate2
-{
-validate_PageTitle=Webview Ruby Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0995
-};
-validate4
-{
-validate_Result=true
-};
-validate5
-{
-validate_Screenshot=VT200_0995
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Manual Compliance Ruby Specs
-};
-validate2
-{
-validate_PageTitle=Webview Ruby Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0999
-};
-validate4
-{
-validate_Result=true
-};
-validate5
-{
-validate_Screenshot=VT200_0999
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Manual Compliance Ruby Specs
-};
-validate2
-{
-validate_PageTitle=Webview Ruby Test
-};
-validate3
-{
-validate_Text_Exists=VT200-1000
-};
-validate4
-{
-validate_Result=true
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Manual Compliance Ruby Specs
-};
-validate2
-{
-validate_PageTitle=Webview Ruby Test
-};
-validate3
-{
-validate_Text_Exists=VT200-1000
-};
-validate4
-{
-validate_Result=false
-};
-validate5
-{
-validate_Screenshot=VT200_1000
-};</t>
-  </si>
-  <si>
-    <t xml:space="preserve">validate1
-{
-validate_PageTitle=Manual Compliance Ruby Specs
-};
-validate2
-{
-validate_PageTitle=Webview Ruby Test
-};
-validate3
-{
-validate_Text_Exists=VT200-1003
-};
-validate4
-{
-validate_Result=true
-};
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">validate1
-{
-validate_PageTitle=Manual Compliance Ruby Specs
-};
-validate2
-{
-validate_PageTitle=Webview Ruby Test
-};
-validate3
-{
-validate_Text_Exists=VT200-1004
-};
-validate4
-{
-validate_Result=1. enable_web_plugins set value is 0
-validate_Result=2. WebView enableWebPlugins value is true
-};
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">validate1
-{
-validate_PageTitle=Manual Compliance Ruby Specs
-};
-validate2
-{
-validate_PageTitle=Webview Ruby Test
-};
-validate3
-{
-validate_Text_Exists=VT200-1004
-};
-validate4
-{
-validate_Result=1. enable_web_plugins set value is 0
-validate_Result=2. WebView enableWebPlugins value is false
-};
-</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Manual Compliance Ruby Specs
-};
-validate2
-{
-validate_PageTitle=Webview Ruby Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0976
-};
-validate5
-{
-validate_Text_Exists=VT200-0978
-};
-validate6
-{
-validate_Result=http://127.0.0.1
-validate_Result=app/WebviewNew/Page4.html
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Manual Compliance Ruby Specs
-};
-validate2
-{
-validate_PageTitle=Webview Ruby Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0976
-};
-validate4
-{
-validate_Text_Exists=VT200-0979
-};
-validate5
-{
-validate_Result=http://127.0.0.1:
-validate_Result=app/WebviewTest/Page1.html
-};</t>
-  </si>
-  <si>
-    <t xml:space="preserve">validate1
-{
-validate_PageTitle=Manual Compliance Ruby Specs
-};
-validate2
-{
-validate_PageTitle=Webview Ruby Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0980
-};
-validate5
-{
-validate_Alert=Hello
-};
-</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Manual Compliance Ruby Specs
-};
-validate2
-{
-validate_PageTitle=Webview Ruby Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0976
-};
-validate4
-{
-validate_Text_Exists=VT200-0981
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Manual Compliance Ruby Specs
-};
-validate2
-{
-validate_PageTitle=Webview Ruby Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0976
-};
-validate4
-{
-validate_Text_Exists=VT200-0985
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Manual Compliance Ruby Specs
-};
-validate2
-{
-validate_PageTitle=Webview Ruby Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0976
-};
-validate4
-{
-validate_Text_Exists=VT200-0985
-};
-validate6
-{
-validate_Text_Exists=VT200-0986
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Manual Compliance Ruby Specs
-};
-validate2
-{
-validate_PageTitle=Webview Ruby Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0976
-};
-validate4
-{
-validate_Text_Exists=VT200-0983
-};
-validate5
-{
-validate_Result=true
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Manual Compliance Ruby Specs
-};
-validate2
-{
-validate_PageTitle=Webview Ruby Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0976
-};
-validate4
-{
-validate_Text_Exists=VT200-0977
-};
-validate5
-{
-validate_Alert=Active Tab is: 1
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Manual Compliance Ruby Specs
-};
-validate2
-{
-validate_PageTitle=Webview Ruby Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0991
-};
-validate4
-{
-validate_SystemProperties=webviewFramework
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Manual Compliance Ruby Specs
-};
-validate2
-{
-validate_PageTitle=Webview Ruby Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0988
-};
-validate4
-{
-validate_Result=true
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Manual Compliance Ruby Specs
-};
-validate2
-{
-validate_PageTitle=Webview Ruby Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0989
-};
-validate4
-{
-validate_Result=true
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Manual Compliance Ruby Specs
-};
-validate2
-{
-validate_PageTitle=Webview Ruby Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0990
-};
-validate4
-{
-validate_Result=true
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Manual Compliance Ruby Specs
-};
-validate2
-{
-validate_PageTitle=Webview Ruby Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0990
-};
-validate4
-{
-validate_Result=false
-};</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -1485,18 +1480,18 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="8.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="35.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="40.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="6.02265625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="1" max="1" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="35" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="40.7109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="35.25" thickBot="1">
@@ -1558,14 +1553,12 @@
         <v>34</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:12" ht="203.25" thickBot="1">
@@ -1589,12 +1582,10 @@
         <v>33</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I3" s="2"/>
-      <c r="J3" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:12" ht="248.25" thickBot="1">
@@ -1616,12 +1607,10 @@
         <v>42</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I4" s="2"/>
-      <c r="J4" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:12" ht="293.25" thickBot="1">
@@ -1642,15 +1631,13 @@
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I5" s="2"/>
-      <c r="J5" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:12" ht="225.75" thickBot="1">
@@ -1674,12 +1661,10 @@
         <v>35</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I6" s="2"/>
-      <c r="J6" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:12" ht="225.75" thickBot="1">
@@ -1700,15 +1685,13 @@
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I7" s="2"/>
-      <c r="J7" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:12" ht="225.75" thickBot="1">
@@ -1730,7 +1713,7 @@
         <v>37</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -1755,7 +1738,7 @@
         <v>41</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1780,7 +1763,7 @@
         <v>36</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -1807,12 +1790,10 @@
         <v>40</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I11" s="2"/>
-      <c r="J11" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:12" ht="214.5" thickBot="1">
@@ -1836,12 +1817,10 @@
         <v>39</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I12" s="2"/>
-      <c r="J12" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:12" ht="214.5" thickBot="1">
@@ -1863,12 +1842,10 @@
         <v>39</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I13" s="2"/>
-      <c r="J13" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:12" ht="259.5" thickBot="1">
@@ -1892,12 +1869,10 @@
         <v>51</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I14" s="2"/>
-      <c r="J14" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:12" ht="259.5" thickBot="1">
@@ -1921,12 +1896,10 @@
         <v>52</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="I15" s="2"/>
-      <c r="J15" s="2" t="s">
-        <v>86</v>
-      </c>
+      <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:12" ht="203.25" thickBot="1">
@@ -1950,12 +1923,10 @@
         <v>38</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I16" s="2"/>
-      <c r="J16" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" ht="259.5" thickBot="1">
@@ -1979,12 +1950,10 @@
         <v>53</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I17" s="2"/>
-      <c r="J17" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:11" ht="304.5" thickBot="1">
@@ -2008,12 +1977,10 @@
         <v>54</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I18" s="2"/>
-      <c r="J18" s="2" t="s">
-        <v>86</v>
-      </c>
+      <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" ht="409.6" thickBot="1">
@@ -2034,18 +2001,16 @@
         <v>1</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I19" s="2"/>
-      <c r="J19" s="2" t="s">
-        <v>86</v>
-      </c>
+      <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" ht="270.75" thickBot="1">
+    <row r="20" spans="1:11" ht="338.25" thickBot="1">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2063,15 +2028,13 @@
         <v>1</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I20" s="2"/>
-      <c r="J20" s="2" t="s">
-        <v>86</v>
-      </c>
+      <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11" ht="270.75" thickBot="1">
@@ -2092,15 +2055,13 @@
         <v>1</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="I21" s="2"/>
-      <c r="J21" s="2" t="s">
-        <v>86</v>
-      </c>
+      <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
     <row r="22" spans="1:11" ht="180.75" thickBot="1">
@@ -2122,12 +2083,10 @@
         <v>45</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I22" s="2"/>
-      <c r="J22" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
     <row r="23" spans="1:11" ht="180.75" thickBot="1">
@@ -2149,12 +2108,10 @@
         <v>48</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I23" s="2"/>
-      <c r="J23" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
     <row r="24" spans="1:11" ht="180.75" thickBot="1">
@@ -2176,12 +2133,10 @@
         <v>49</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="I24" s="2"/>
-      <c r="J24" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
     <row r="25" spans="1:11" ht="180.75" thickBot="1">
@@ -2203,12 +2158,10 @@
         <v>50</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I25" s="2"/>
-      <c r="J25" s="2" t="s">
-        <v>85</v>
-      </c>
+      <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
     <row r="26" spans="1:11" ht="180.75" thickBot="1">
@@ -2230,7 +2183,7 @@
         <v>50</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>

</xml_diff>